<commit_message>
Broke up into multiple files
</commit_message>
<xml_diff>
--- a/Scripts/plan.xlsx
+++ b/Scripts/plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28100" yWindow="700" windowWidth="33840" windowHeight="23040"/>
+    <workbookView xWindow="520" yWindow="460" windowWidth="28680" windowHeight="27860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="118">
   <si>
     <t>Lesson #</t>
   </si>
@@ -382,6 +382,9 @@
   </si>
   <si>
     <t>2-5 capsense motor</t>
+  </si>
+  <si>
+    <t>add a description of how a pwm works… and</t>
   </si>
 </sst>
 </file>
@@ -447,12 +450,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -476,9 +478,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -487,6 +486,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -805,17 +816,17 @@
   <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="9" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="9" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
@@ -826,42 +837,42 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="14" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -870,32 +881,32 @@
       <c r="C2" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="6">
+      <c r="D2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="5">
         <v>781</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <f>507/60</f>
         <v>8.4499999999999993</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6" t="s">
+      <c r="H2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
@@ -904,32 +915,32 @@
       <c r="C3" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" s="6">
+      <c r="D3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="5">
         <v>830</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="10">
         <f>416/60</f>
         <v>6.9333333333333336</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6" t="s">
+      <c r="H3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
@@ -938,32 +949,32 @@
       <c r="C4" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="D4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="5">
         <v>1196</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <f>666/60</f>
         <v>11.1</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6" t="s">
+      <c r="H4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
@@ -972,748 +983,759 @@
       <c r="C5" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" s="6">
+      <c r="D5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="5">
         <v>555</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <f>340/60</f>
         <v>5.666666666666667</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6" t="s">
+      <c r="H5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="6">
-        <v>1600</v>
-      </c>
-      <c r="G6" s="11">
+      <c r="D6" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="5">
+        <v>711</v>
+      </c>
+      <c r="G6" s="10">
         <f t="shared" ref="G6:G24" si="0">(F6/1.75)/60</f>
-        <v>15.238095238095239</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6" t="s">
+        <v>6.7714285714285714</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B7" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="16">
+        <v>971</v>
+      </c>
+      <c r="G7" s="17">
+        <f t="shared" si="0"/>
+        <v>9.2476190476190485</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="16">
+        <v>739</v>
+      </c>
+      <c r="G8" s="17">
+        <f t="shared" si="0"/>
+        <v>7.038095238095238</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="16">
+        <v>1631</v>
+      </c>
+      <c r="G9" s="17">
+        <f t="shared" si="0"/>
+        <v>15.533333333333333</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="16">
+        <v>609</v>
+      </c>
+      <c r="G10" s="17">
+        <f t="shared" si="0"/>
+        <v>5.8</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="16">
+        <v>814</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="0"/>
+        <v>7.7523809523809524</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="16">
+        <v>856</v>
+      </c>
+      <c r="G12" s="17">
+        <f t="shared" si="0"/>
+        <v>8.1523809523809536</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="5">
+        <v>910</v>
+      </c>
+      <c r="G13" s="10">
+        <f t="shared" si="0"/>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="5">
+        <v>469</v>
+      </c>
+      <c r="G14" s="10">
+        <f t="shared" si="0"/>
+        <v>4.4666666666666668</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="11">
+      <c r="E15" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6" t="s">
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="6">
-        <v>1954</v>
-      </c>
-      <c r="G8" s="11">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1973</v>
+      </c>
+      <c r="G16" s="10">
         <f t="shared" si="0"/>
-        <v>18.609523809523811</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6" t="s">
+        <v>18.790476190476188</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E9" s="13" t="s">
+      <c r="L16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1515</v>
+      </c>
+      <c r="G17" s="10">
+        <f t="shared" si="0"/>
+        <v>14.428571428571427</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1383</v>
+      </c>
+      <c r="G18" s="10">
+        <f t="shared" si="0"/>
+        <v>13.171428571428573</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="6">
+        <v>2227</v>
+      </c>
+      <c r="G19" s="10">
+        <f t="shared" si="0"/>
+        <v>21.209523809523812</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="11">
+      <c r="E20" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6" t="s">
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F10" s="6">
-        <v>1478</v>
-      </c>
-      <c r="G10" s="11">
-        <f t="shared" si="0"/>
-        <v>14.076190476190476</v>
-      </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E11" s="13" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="11">
+      <c r="E22" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6" t="s">
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="6">
-        <v>856</v>
-      </c>
-      <c r="G12" s="11">
-        <f t="shared" si="0"/>
-        <v>8.1523809523809536</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="6">
-        <v>1392</v>
-      </c>
-      <c r="G13" s="11">
-        <f t="shared" si="0"/>
-        <v>13.257142857142858</v>
-      </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B14" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="7">
-        <v>1973</v>
-      </c>
-      <c r="G16" s="11">
-        <f t="shared" si="0"/>
-        <v>18.790476190476188</v>
-      </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="L16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="7">
-        <v>1515</v>
-      </c>
-      <c r="G17" s="11">
-        <f t="shared" si="0"/>
-        <v>14.428571428571427</v>
-      </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="7">
-        <v>1383</v>
-      </c>
-      <c r="G18" s="11">
-        <f t="shared" si="0"/>
-        <v>13.171428571428573</v>
-      </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="7">
-        <v>2227</v>
-      </c>
-      <c r="G19" s="11">
-        <f t="shared" si="0"/>
-        <v>21.209523809523812</v>
-      </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="L19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="7" t="s">
+      <c r="C24" s="4"/>
+      <c r="D24" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24" s="7">
+      <c r="E24" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="6">
         <v>1384</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="10">
         <f t="shared" si="0"/>
         <v>13.180952380952382</v>
       </c>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="6" t="s">
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="7" t="s">
+      <c r="C25" s="4"/>
+      <c r="D25" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="6" t="s">
+      <c r="F25" s="6"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
       <c r="L26" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
       <c r="L27" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
       <c r="L28" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
       <c r="L29" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
       <c r="L32" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
       <c r="L33" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
       <c r="L34" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B35" t="s">
@@ -1722,17 +1744,17 @@
       <c r="C35" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B36" t="s">
@@ -1741,17 +1763,17 @@
       <c r="C36" t="s">
         <v>61</v>
       </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B37" t="s">
@@ -1760,17 +1782,17 @@
       <c r="C37" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B38" t="s">
@@ -1779,17 +1801,17 @@
       <c r="C38" t="s">
         <v>61</v>
       </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B39" t="s">
@@ -1798,17 +1820,17 @@
       <c r="C39" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B40" t="s">
@@ -1817,17 +1839,17 @@
       <c r="C40" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B41" t="s">
@@ -1836,17 +1858,17 @@
       <c r="C41" t="s">
         <v>62</v>
       </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B42" t="s">
@@ -1855,17 +1877,17 @@
       <c r="C42" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B43" t="s">
@@ -1874,14 +1896,14 @@
       <c r="C43" t="s">
         <v>62</v>
       </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
Updates to the projects
</commit_message>
<xml_diff>
--- a/Scripts/plan.xlsx
+++ b/Scripts/plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="520" yWindow="460" windowWidth="28680" windowHeight="27860"/>
+    <workbookView xWindow="23220" yWindow="460" windowWidth="28680" windowHeight="27860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>Basic Thermistor</t>
   </si>
   <si>
-    <t>3-6</t>
-  </si>
-  <si>
     <t>Basic Motion Sensor</t>
   </si>
   <si>
@@ -315,9 +312,6 @@
     <t>Make the first Remote Control Project (uart)</t>
   </si>
   <si>
-    <t>3-6b</t>
-  </si>
-  <si>
     <t>2-3a</t>
   </si>
   <si>
@@ -360,9 +354,6 @@
     <t>3-5-basictherm</t>
   </si>
   <si>
-    <t>3-6-basicmotion</t>
-  </si>
-  <si>
     <t>3-3-simpleblecentral</t>
   </si>
   <si>
@@ -397,6 +388,15 @@
   </si>
   <si>
     <t>add kill switch to the main controller</t>
+  </si>
+  <si>
+    <t>3-5a</t>
+  </si>
+  <si>
+    <t>3-5b</t>
+  </si>
+  <si>
+    <t>3-5-basicmotion</t>
   </si>
 </sst>
 </file>
@@ -831,7 +831,7 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -856,34 +856,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="J1" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>68</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -894,13 +894,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F2" s="5">
         <v>781</v>
@@ -910,14 +910,14 @@
         <v>8.4499999999999993</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -928,13 +928,13 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" s="5">
         <v>830</v>
@@ -944,14 +944,14 @@
         <v>6.9333333333333336</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -962,13 +962,13 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" s="5">
         <v>1196</v>
@@ -978,14 +978,14 @@
         <v>11.1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -996,13 +996,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" s="5">
         <v>555</v>
@@ -1012,28 +1012,28 @@
         <v>5.666666666666667</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F6" s="5">
         <v>711</v>
@@ -1046,21 +1046,21 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7" s="16">
         <v>971</v>
@@ -1073,21 +1073,21 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8" s="16">
         <v>739</v>
@@ -1100,24 +1100,24 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" s="16">
         <v>1631</v>
@@ -1130,21 +1130,21 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" s="16">
         <v>609</v>
@@ -1157,21 +1157,21 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F11" s="16">
         <v>814</v>
@@ -1184,21 +1184,21 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F12" s="16">
         <v>722</v>
@@ -1211,21 +1211,21 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" t="s">
         <v>118</v>
       </c>
-      <c r="B13" t="s">
-        <v>121</v>
-      </c>
       <c r="D13" s="13" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F13" s="16">
         <v>761</v>
@@ -1238,21 +1238,21 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F14" s="5">
         <v>910</v>
@@ -1265,21 +1265,21 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F15" s="5">
         <v>469</v>
@@ -1292,22 +1292,22 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="10">
@@ -1318,7 +1318,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1330,10 +1330,10 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="10">
@@ -1344,7 +1344,7 @@
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1352,14 +1352,14 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F18" s="6">
         <v>1973</v>
@@ -1372,25 +1372,25 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F19" s="6">
         <v>1515</v>
@@ -1403,22 +1403,22 @@
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F20" s="6">
         <v>1383</v>
@@ -1431,22 +1431,22 @@
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F21" s="6">
         <v>2227</v>
@@ -1459,25 +1459,25 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="10"/>
@@ -1488,17 +1488,17 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="10">
@@ -1509,22 +1509,22 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="10"/>
@@ -1535,17 +1535,17 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="6" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F25" s="6">
         <v>1384</v>
@@ -1558,22 +1558,22 @@
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="8"/>
@@ -1581,18 +1581,18 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="C27" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -1603,18 +1603,18 @@
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="C28" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -1625,18 +1625,18 @@
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="C29" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -1647,18 +1647,18 @@
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="C30" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -1669,18 +1669,18 @@
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="C31" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -1693,13 +1693,13 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="C32" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -1712,13 +1712,13 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="C33" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -1729,18 +1729,18 @@
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
       <c r="L33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="C34" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -1751,18 +1751,18 @@
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
       <c r="L34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="C35" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -1773,18 +1773,18 @@
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
       <c r="L35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -1797,13 +1797,13 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
@@ -1816,13 +1816,13 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
@@ -1835,13 +1835,13 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -1873,13 +1873,13 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -1892,13 +1892,13 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -1911,13 +1911,13 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -1930,13 +1930,13 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" t="s">
         <v>47</v>
       </c>
-      <c r="B44" t="s">
-        <v>48</v>
-      </c>
       <c r="C44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>

</xml_diff>

<commit_message>
added the ble remote control uart based robot controller
</commit_message>
<xml_diff>
--- a/Scripts/plan.xlsx
+++ b/Scripts/plan.xlsx
@@ -430,7 +430,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,12 +440,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -462,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -491,9 +485,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -831,7 +822,7 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,37 +843,37 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1059,13 +1050,13 @@
       <c r="D7" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="16">
+      <c r="E7" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="15">
         <v>971</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="16">
         <f t="shared" si="0"/>
         <v>9.2476190476190485</v>
       </c>
@@ -1086,13 +1077,13 @@
       <c r="D8" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="16">
+      <c r="E8" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="15">
         <v>739</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="16">
         <f t="shared" si="0"/>
         <v>7.038095238095238</v>
       </c>
@@ -1116,13 +1107,13 @@
       <c r="D9" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="16">
+      <c r="E9" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="15">
         <v>1631</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="16">
         <f t="shared" si="0"/>
         <v>15.533333333333333</v>
       </c>
@@ -1143,13 +1134,13 @@
       <c r="D10" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" s="16">
+      <c r="E10" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="15">
         <v>609</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="16">
         <f t="shared" si="0"/>
         <v>5.8</v>
       </c>
@@ -1170,13 +1161,13 @@
       <c r="D11" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="16">
+      <c r="E11" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="15">
         <v>814</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="16">
         <f t="shared" si="0"/>
         <v>7.7523809523809524</v>
       </c>
@@ -1194,16 +1185,16 @@
       <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="16">
+      <c r="E12" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="15">
         <v>722</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="16">
         <f t="shared" ref="G12" si="1">(F12/1.75)/60</f>
         <v>6.8761904761904757</v>
       </c>
@@ -1221,16 +1212,16 @@
       <c r="B13" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="16">
+      <c r="E13" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="15">
         <v>761</v>
       </c>
-      <c r="G13" s="17">
+      <c r="G13" s="16">
         <f t="shared" si="0"/>
         <v>7.2476190476190476</v>
       </c>
@@ -1296,7 +1287,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1478,11 +1469,16 @@
       <c r="D22" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="10"/>
+      <c r="E22" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="6">
+        <v>810</v>
+      </c>
+      <c r="G22" s="10">
+        <f t="shared" si="0"/>
+        <v>7.7142857142857135</v>
+      </c>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>

</xml_diff>

<commit_message>
first crack at 3-4
</commit_message>
<xml_diff>
--- a/Scripts/plan.xlsx
+++ b/Scripts/plan.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="121">
   <si>
     <t>Lesson #</t>
   </si>
@@ -288,21 +288,12 @@
     <t>3-3a</t>
   </si>
   <si>
-    <t>3-4b</t>
-  </si>
-  <si>
-    <t>3-4a</t>
-  </si>
-  <si>
     <t>Simple BLE Custom Service</t>
   </si>
   <si>
     <t>Add ble to the main controller</t>
   </si>
   <si>
-    <t>BLE CapSense Remote control of LED Service 3-2a</t>
-  </si>
-  <si>
     <t>Simple BLE Central control of LED Service 3-2a</t>
   </si>
   <si>
@@ -397,6 +388,12 @@
   </si>
   <si>
     <t>3-5-basicmotion</t>
+  </si>
+  <si>
+    <t>3-4</t>
+  </si>
+  <si>
+    <t>rc3-4 CapSense</t>
   </si>
 </sst>
 </file>
@@ -819,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1015,7 +1012,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -1030,7 +1027,7 @@
         <v>711</v>
       </c>
       <c r="G6" s="10">
-        <f t="shared" ref="G6:G25" si="0">(F6/1.75)/60</f>
+        <f t="shared" ref="G6:G24" si="0">(F6/1.75)/60</f>
         <v>6.7714285714285714</v>
       </c>
       <c r="H6" s="5"/>
@@ -1042,13 +1039,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
         <v>76</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>70</v>
@@ -1069,7 +1066,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -1094,18 +1091,18 @@
         <v>77</v>
       </c>
       <c r="L8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
         <v>75</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>70</v>
@@ -1126,7 +1123,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
@@ -1153,13 +1150,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>70</v>
@@ -1180,13 +1177,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>70</v>
@@ -1207,13 +1204,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" t="s">
         <v>115</v>
       </c>
-      <c r="B13" t="s">
-        <v>118</v>
-      </c>
       <c r="D13" s="12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>70</v>
@@ -1234,13 +1231,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>70</v>
@@ -1261,13 +1258,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B15" t="s">
         <v>73</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>70</v>
@@ -1288,14 +1285,14 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>70</v>
@@ -1349,7 +1346,7 @@
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>70</v>
@@ -1376,11 +1373,11 @@
         <v>81</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>70</v>
@@ -1404,11 +1401,11 @@
         <v>82</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>70</v>
@@ -1432,11 +1429,11 @@
         <v>84</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>70</v>
@@ -1463,11 +1460,11 @@
         <v>83</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>70</v>
@@ -1486,72 +1483,69 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="F23" s="6"/>
-      <c r="G23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G23" s="10"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="5" t="s">
-        <v>77</v>
-      </c>
+      <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>91</v>
+        <v>19</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="10"/>
+        <v>118</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" s="6">
+        <v>1384</v>
+      </c>
+      <c r="G24" s="10">
+        <f t="shared" si="0"/>
+        <v>13.180952380952382</v>
+      </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="5"/>
+      <c r="K24" s="5" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F25" s="6">
-        <v>1384</v>
-      </c>
-      <c r="G25" s="10">
-        <f t="shared" si="0"/>
-        <v>13.180952380952382</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="8"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
@@ -1561,33 +1555,32 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>69</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="8"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
-      <c r="K26" s="5" t="s">
-        <v>77</v>
+      <c r="K26" s="6"/>
+      <c r="L26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>59</v>
@@ -1606,10 +1599,10 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>59</v>
@@ -1628,10 +1621,10 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>59</v>
@@ -1650,13 +1643,13 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -1666,16 +1659,13 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
-      <c r="L30" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>57</v>
@@ -1691,13 +1681,13 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -1707,13 +1697,16 @@
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
+      <c r="L32" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>58</v>
@@ -1732,10 +1725,10 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>58</v>
@@ -1753,33 +1746,30 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="A35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" t="s">
-        <v>60</v>
-      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C36" t="s">
         <v>58</v>
@@ -1795,10 +1785,10 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
         <v>58</v>
@@ -1814,10 +1804,10 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C38" t="s">
         <v>58</v>
@@ -1833,13 +1823,13 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
@@ -1852,10 +1842,10 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C40" t="s">
         <v>59</v>
@@ -1871,10 +1861,10 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C41" t="s">
         <v>59</v>
@@ -1890,10 +1880,10 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C42" t="s">
         <v>59</v>
@@ -1909,10 +1899,10 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C43" t="s">
         <v>59</v>
@@ -1926,25 +1916,6 @@
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44" t="s">
-        <v>59</v>
-      </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
remote control motion sensor
</commit_message>
<xml_diff>
--- a/Scripts/plan.xlsx
+++ b/Scripts/plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="28680" windowHeight="17540"/>
+    <workbookView xWindow="22520" yWindow="5860" windowWidth="28680" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="121">
   <si>
     <t>Lesson #</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>Script Words</t>
+  </si>
+  <si>
+    <t>rc3-5b-Motion</t>
   </si>
 </sst>
 </file>
@@ -810,7 +813,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F24"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1463,7 +1466,7 @@
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="6" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="8"/>

</xml_diff>